<commit_message>
-Meh update the data to give more reasonable output. Will think on this more when we get more constraints built in. Semi accurate with optimal run taking 180911 frames (50.18m)
</commit_message>
<xml_diff>
--- a/data/times.xlsx
+++ b/data/times.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="146">
   <si>
     <t>level</t>
   </si>
@@ -26761,52 +26761,52 @@
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="3"/>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="3"/>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>29</v>
@@ -26815,425 +26815,423 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>140</v>
+        <v>29</v>
       </c>
       <c r="C13" s="3"/>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>139</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="C14" s="3"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C16" s="3"/>
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C17" s="3"/>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C18" s="3"/>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C19" s="3"/>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C20" s="3"/>
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>139</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C21" s="3"/>
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C22" s="3"/>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="3"/>
+        <v>51</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C24" s="3"/>
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C25" s="3"/>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C26" s="3"/>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>141</v>
+        <v>57</v>
       </c>
       <c r="C27" s="3"/>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>139</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="C28" s="3"/>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C29" s="3"/>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
       <c r="C30" s="3"/>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>142</v>
+        <v>65</v>
       </c>
       <c r="C32" s="3"/>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C33" s="3"/>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C34" s="3"/>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C35" s="3"/>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>76</v>
+        <v>142</v>
       </c>
       <c r="C36" s="3"/>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>143</v>
+        <v>73</v>
       </c>
       <c r="C37" s="3"/>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C38" s="3"/>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C39" s="3"/>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>139</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="C40" s="3"/>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>89</v>
+        <v>143</v>
       </c>
       <c r="C41" s="3"/>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C42" s="3"/>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C43" s="3"/>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C44" s="3"/>
+        <v>84</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C45" s="3"/>
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C46" s="3"/>
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>144</v>
+        <v>85</v>
       </c>
       <c r="C47" s="3"/>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>139</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="C48" s="3"/>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="C49" s="3"/>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="C50" s="3"/>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="C51" s="3"/>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="C52" s="3"/>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="C53" s="3"/>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="C54" s="3"/>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="C55" s="3"/>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>145</v>
+        <v>95</v>
       </c>
       <c r="C56" s="3"/>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
       <c r="C57" s="3"/>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>139</v>
@@ -27241,155 +27239,205 @@
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="C59" s="3"/>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="C60" s="3"/>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="C61" s="3"/>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="C62" s="3"/>
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="C63" s="3"/>
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="C64" s="3"/>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="C65" s="3"/>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="C66" s="3"/>
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="C67" s="3"/>
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C68" s="3"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C70" s="3"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C71" s="3"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C72" s="3"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C73" s="3"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C74" s="3"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C75" s="3"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C76" s="3"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C77" s="3"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C78" s="3"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C79" s="3"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B80" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C80" s="5" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="3"/>
-      <c r="B69" s="3"/>
-      <c r="C69" s="3"/>
-    </row>
-    <row r="70">
-      <c r="A70" s="3"/>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-    </row>
-    <row r="71">
-      <c r="A71" s="3"/>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-    </row>
-    <row r="72">
-      <c r="A72" s="3"/>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-    </row>
-    <row r="73">
-      <c r="A73" s="3"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
-    </row>
-    <row r="74">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
-    </row>
-    <row r="75">
-      <c r="A75" s="3"/>
-      <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
-    </row>
-    <row r="76">
-      <c r="A76" s="3"/>
-      <c r="B76" s="3"/>
-      <c r="C76" s="3"/>
-    </row>
-    <row r="77">
-      <c r="A77" s="3"/>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
-    </row>
-    <row r="78">
-      <c r="A78" s="3"/>
-      <c r="B78" s="3"/>
-      <c r="C78" s="3"/>
-    </row>
-    <row r="79">
-      <c r="A79" s="3"/>
-      <c r="B79" s="3"/>
-      <c r="C79" s="3"/>
-    </row>
-    <row r="80">
-      <c r="A80" s="3"/>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
     </row>
     <row r="81">
       <c r="A81" s="3"/>
@@ -31966,6 +32014,66 @@
       <c r="B995" s="3"/>
       <c r="C995" s="3"/>
     </row>
+    <row r="996">
+      <c r="A996" s="3"/>
+      <c r="B996" s="3"/>
+      <c r="C996" s="3"/>
+    </row>
+    <row r="997">
+      <c r="A997" s="3"/>
+      <c r="B997" s="3"/>
+      <c r="C997" s="3"/>
+    </row>
+    <row r="998">
+      <c r="A998" s="3"/>
+      <c r="B998" s="3"/>
+      <c r="C998" s="3"/>
+    </row>
+    <row r="999">
+      <c r="A999" s="3"/>
+      <c r="B999" s="3"/>
+      <c r="C999" s="3"/>
+    </row>
+    <row r="1000">
+      <c r="A1000" s="3"/>
+      <c r="B1000" s="3"/>
+      <c r="C1000" s="3"/>
+    </row>
+    <row r="1001">
+      <c r="A1001" s="3"/>
+      <c r="B1001" s="3"/>
+      <c r="C1001" s="3"/>
+    </row>
+    <row r="1002">
+      <c r="A1002" s="3"/>
+      <c r="B1002" s="3"/>
+      <c r="C1002" s="3"/>
+    </row>
+    <row r="1003">
+      <c r="A1003" s="3"/>
+      <c r="B1003" s="3"/>
+      <c r="C1003" s="3"/>
+    </row>
+    <row r="1004">
+      <c r="A1004" s="3"/>
+      <c r="B1004" s="3"/>
+      <c r="C1004" s="3"/>
+    </row>
+    <row r="1005">
+      <c r="A1005" s="3"/>
+      <c r="B1005" s="3"/>
+      <c r="C1005" s="3"/>
+    </row>
+    <row r="1006">
+      <c r="A1006" s="3"/>
+      <c r="B1006" s="3"/>
+      <c r="C1006" s="3"/>
+    </row>
+    <row r="1007">
+      <c r="A1007" s="3"/>
+      <c r="B1007" s="3"/>
+      <c r="C1007" s="3"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update item usage. add logging
</commit_message>
<xml_diff>
--- a/data/times.xlsx
+++ b/data/times.xlsx
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1095" uniqueCount="246">
   <si>
     <t>This spreadsheet is intended to capture all times for levels given some input and expected output.</t>
   </si>
@@ -541,6 +541,9 @@
   </si>
   <si>
     <t>7-F1</t>
+  </si>
+  <si>
+    <t>(exit with tanooki, but who cares :D)</t>
   </si>
   <si>
     <t>7-6</t>
@@ -1242,13 +1245,13 @@
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2">
@@ -1366,7 +1369,7 @@
         <v>46</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C14" s="10"/>
     </row>
@@ -1514,7 +1517,7 @@
         <v>82</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C30" s="10"/>
     </row>
@@ -1570,7 +1573,7 @@
         <v>91</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C36" s="10"/>
     </row>
@@ -1615,7 +1618,7 @@
         <v>104</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C41" s="10"/>
     </row>
@@ -1761,7 +1764,7 @@
         <v>128</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C57" s="10"/>
     </row>
@@ -1823,7 +1826,7 @@
     </row>
     <row r="64">
       <c r="A64" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>149</v>
@@ -1832,46 +1835,46 @@
     </row>
     <row r="65">
       <c r="A65" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="C65" s="10"/>
     </row>
     <row r="66">
       <c r="A66" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C66" s="10"/>
     </row>
     <row r="67">
       <c r="A67" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C67" s="10"/>
     </row>
     <row r="68">
       <c r="A68" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C68" s="10"/>
     </row>
     <row r="69">
       <c r="A69" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>93</v>
@@ -1879,10 +1882,10 @@
     </row>
     <row r="70">
       <c r="A70" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>93</v>
@@ -1890,10 +1893,10 @@
     </row>
     <row r="71">
       <c r="A71" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>93</v>
@@ -1901,37 +1904,37 @@
     </row>
     <row r="72">
       <c r="A72" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B72" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>174</v>
       </c>
       <c r="C72" s="10"/>
     </row>
     <row r="73">
       <c r="A73" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B73" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>175</v>
       </c>
       <c r="C73" s="10"/>
     </row>
     <row r="74">
       <c r="A74" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C74" s="10"/>
     </row>
     <row r="75">
       <c r="A75" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B75" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>178</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>93</v>
@@ -1939,37 +1942,37 @@
     </row>
     <row r="76">
       <c r="A76" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B76" s="3" t="s">
         <v>180</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>179</v>
       </c>
       <c r="C76" s="10"/>
     </row>
     <row r="77">
       <c r="A77" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C77" s="10"/>
     </row>
     <row r="78">
       <c r="A78" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C78" s="10"/>
     </row>
     <row r="79">
       <c r="A79" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>93</v>
@@ -1977,10 +1980,10 @@
     </row>
     <row r="80">
       <c r="A80" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B80" s="3" t="s">
         <v>194</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>193</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>93</v>
@@ -6650,12 +6653,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -6663,42 +6666,42 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>216</v>
-      </c>
       <c r="K4" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5">
@@ -6709,7 +6712,7 @@
         <v>2.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E5" s="1">
         <v>0.0</v>
@@ -6718,7 +6721,7 @@
         <v>2.0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="I5" s="1">
         <v>0.0</v>
@@ -6727,7 +6730,7 @@
         <v>2.0</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6">
@@ -6738,7 +6741,7 @@
         <v>2.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E6" s="1">
         <v>2.0</v>
@@ -6747,7 +6750,7 @@
         <v>2.0</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="I6" s="1">
         <v>2.0</v>
@@ -6756,7 +6759,7 @@
         <v>2.0</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7">
@@ -6767,7 +6770,7 @@
         <v>12.0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E7" s="1">
         <v>12.0</v>
@@ -6776,7 +6779,7 @@
         <v>12.0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I7" s="1">
         <v>12.0</v>
@@ -6785,7 +6788,7 @@
         <v>12.0</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8">
@@ -6796,7 +6799,7 @@
         <v>13.0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E8" s="1">
         <v>13.0</v>
@@ -6805,7 +6808,7 @@
         <v>13.0</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="I8" s="1">
         <v>11.0</v>
@@ -6814,7 +6817,7 @@
         <v>11.0</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9">
@@ -6825,7 +6828,7 @@
         <v>-8.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E9" s="1">
         <v>-10.0</v>
@@ -6834,7 +6837,7 @@
         <v>-8.0</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I9" s="1">
         <v>-10.0</v>
@@ -6843,7 +6846,7 @@
         <v>-8.0</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10">
@@ -6854,7 +6857,7 @@
         <v>30.5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E10" s="1">
         <v>30.5</v>
@@ -6863,7 +6866,7 @@
         <v>30.5</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="I10" s="1">
         <v>30.5</v>
@@ -6872,7 +6875,7 @@
         <v>30.5</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11">
@@ -6883,7 +6886,7 @@
         <v>25.5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E11" s="1">
         <v>25.5</v>
@@ -6892,7 +6895,7 @@
         <v>25.5</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="I11" s="1">
         <v>25.5</v>
@@ -6901,7 +6904,7 @@
         <v>25.5</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12">
@@ -6912,7 +6915,7 @@
         <v>1.0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E12" s="1">
         <v>1.0</v>
@@ -6921,7 +6924,7 @@
         <v>1.0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13">
@@ -6932,7 +6935,7 @@
         <v>-3.0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E13" s="1">
         <v>-3.0</v>
@@ -6941,7 +6944,7 @@
         <v>-3.0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14">
@@ -6952,7 +6955,7 @@
         <v>-1.5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E14" s="1">
         <v>-1.5</v>
@@ -6961,7 +6964,7 @@
         <v>-1.5</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15">
@@ -6972,7 +6975,7 @@
         <v>1.0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E15" s="1">
         <v>1.0</v>
@@ -6981,7 +6984,7 @@
         <v>1.0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I15" s="1">
         <v>1.0</v>
@@ -6990,7 +6993,7 @@
         <v>1.0</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16">
@@ -7001,7 +7004,7 @@
         <v>-3.0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E16" s="1">
         <v>-3.0</v>
@@ -7010,7 +7013,7 @@
         <v>-3.0</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I16" s="1">
         <v>-3.0</v>
@@ -7019,7 +7022,7 @@
         <v>-3.0</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17">
@@ -7030,7 +7033,7 @@
         <v>-2.0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E17" s="1">
         <v>-2.0</v>
@@ -7039,7 +7042,7 @@
         <v>-2.0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="18">
@@ -7050,7 +7053,7 @@
         <v>-1.0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E18" s="1">
         <v>-1.0</v>
@@ -7059,7 +7062,7 @@
         <v>-1.0</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I18" s="1">
         <v>-1.0</v>
@@ -7068,7 +7071,7 @@
         <v>-1.0</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="19">
@@ -7079,7 +7082,7 @@
         <v>-36.25</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E19" s="1">
         <v>-36.0</v>
@@ -7088,10 +7091,10 @@
         <v>-36.0</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="I19" s="1">
         <v>-36.25</v>
@@ -7100,7 +7103,7 @@
         <v>-36.25</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="20">
@@ -7111,7 +7114,7 @@
         <v>-41.0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E20" s="1">
         <v>-40.5</v>
@@ -7120,7 +7123,7 @@
         <v>-40.5</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="I20" s="1">
         <v>-41.0</v>
@@ -7129,7 +7132,7 @@
         <v>-41.0</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="21">
@@ -7142,7 +7145,7 @@
         <v>-8.75</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E21" s="16">
         <f t="shared" ref="E21:F21" si="2">SUM(E5:E20)</f>
@@ -7153,7 +7156,7 @@
         <v>-8</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="I21" s="16">
         <f t="shared" ref="I21:J21" si="3">sum(I5:I20)</f>
@@ -7164,7 +7167,7 @@
         <v>-5.25</v>
       </c>
       <c r="K21" s="17" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -7195,15 +7198,15 @@
   <sheetData>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B3" s="1">
         <v>16.0</v>
@@ -7211,7 +7214,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B4" s="1">
         <v>17.0</v>
@@ -7219,7 +7222,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B5" s="1">
         <f>86-20</f>
@@ -7228,7 +7231,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B6" s="18">
         <f>92+1</f>
@@ -7237,7 +7240,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B7" s="18">
         <f>1817-1785</f>
@@ -7246,7 +7249,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B8" s="1">
         <v>37.0</v>
@@ -7254,7 +7257,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B9" s="18">
         <f>4*60</f>
@@ -7619,7 +7622,28 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="10"/>
+      <c r="A15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="1">
+        <v>10443.0</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="10"/>
@@ -11049,7 +11073,28 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="10"/>
+      <c r="A18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="1">
+        <v>11854.0</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="10"/>
@@ -21156,23 +21201,23 @@
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B17" s="1">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="F17" s="1">
-        <v>2037.0</v>
+        <v>2105.0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18">
@@ -21180,7 +21225,7 @@
         <v>96</v>
       </c>
       <c r="B18" s="1">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>31</v>
@@ -21190,59 +21235,39 @@
         <v>31</v>
       </c>
       <c r="F18" s="1">
+        <v>2037.0</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="1">
         <v>1849.0</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B19" s="5">
-        <v>7.0</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="5">
-        <v>2226.0</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="8"/>
-      <c r="S19" s="8"/>
-      <c r="T19" s="8"/>
-      <c r="U19" s="8"/>
-      <c r="V19" s="8"/>
-      <c r="W19" s="8"/>
-      <c r="X19" s="8"/>
-      <c r="Y19" s="8"/>
-      <c r="Z19" s="8"/>
-      <c r="AA19" s="8"/>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
         <v>96</v>
       </c>
       <c r="B20" s="5">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>16</v>
@@ -21252,10 +21277,10 @@
         <v>25</v>
       </c>
       <c r="F20" s="5">
-        <v>2039.0</v>
+        <v>2226.0</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
@@ -21283,17 +21308,17 @@
         <v>96</v>
       </c>
       <c r="B21" s="5">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>16</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F21" s="5">
-        <v>1903.0</v>
+        <v>2039.0</v>
       </c>
       <c r="G21" s="9" t="s">
         <v>99</v>
@@ -21320,45 +21345,65 @@
       <c r="AA21" s="8"/>
     </row>
     <row r="22">
-      <c r="A22" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B22" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F22" s="1">
-        <v>2057.0</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>101</v>
-      </c>
+      <c r="A22" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="5">
+        <v>1903.0</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+      <c r="T22" s="8"/>
+      <c r="U22" s="8"/>
+      <c r="V22" s="8"/>
+      <c r="W22" s="8"/>
+      <c r="X22" s="8"/>
+      <c r="Y22" s="8"/>
+      <c r="Z22" s="8"/>
+      <c r="AA22" s="8"/>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
         <v>100</v>
       </c>
       <c r="B23" s="1">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F23" s="1">
-        <v>2654.0</v>
+        <v>2057.0</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24">
@@ -21366,20 +21411,20 @@
         <v>100</v>
       </c>
       <c r="B24" s="1">
-        <v>7.0</v>
+        <v>4.0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F24" s="1">
-        <v>2228.0</v>
+        <v>2654.0</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25">
@@ -21387,48 +21432,51 @@
         <v>100</v>
       </c>
       <c r="B25" s="1">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>93</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F25" s="1">
-        <v>2213.0</v>
+        <v>2228.0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B26" s="1">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="E26" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F26" s="1">
-        <v>10039.0</v>
+        <v>2213.0</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B27" s="1">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>31</v>
@@ -21438,15 +21486,15 @@
         <v>31</v>
       </c>
       <c r="F27" s="1">
-        <v>2834.0</v>
+        <v>10039.0</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="3" t="s">
         <v>104</v>
       </c>
       <c r="B28" s="1">
-        <v>8.0</v>
+        <v>4.0</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>31</v>
@@ -21456,18 +21504,15 @@
         <v>31</v>
       </c>
       <c r="F28" s="1">
-        <v>2453.0</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>105</v>
+        <v>2834.0</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="3" t="s">
-        <v>106</v>
+      <c r="A29" s="1" t="s">
+        <v>104</v>
       </c>
       <c r="B29" s="1">
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>31</v>
@@ -21477,15 +21522,18 @@
         <v>31</v>
       </c>
       <c r="F29" s="1">
-        <v>2120.0</v>
+        <v>2453.0</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B30" s="1">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>31</v>
@@ -21495,15 +21543,15 @@
         <v>31</v>
       </c>
       <c r="F30" s="1">
-        <v>5556.0</v>
+        <v>2120.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B31" s="1">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>31</v>
@@ -21513,10 +21561,7 @@
         <v>31</v>
       </c>
       <c r="F31" s="1">
-        <v>12027.0</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>49</v>
+        <v>5556.0</v>
       </c>
     </row>
     <row r="32">
@@ -21524,7 +21569,7 @@
         <v>108</v>
       </c>
       <c r="B32" s="1">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>31</v>
@@ -21534,10 +21579,7 @@
         <v>31</v>
       </c>
       <c r="F32" s="1">
-        <v>11814.0</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>109</v>
+        <v>12027.0</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>49</v>
@@ -21548,7 +21590,7 @@
         <v>108</v>
       </c>
       <c r="B33" s="1">
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>31</v>
@@ -21558,7 +21600,7 @@
         <v>31</v>
       </c>
       <c r="F33" s="1">
-        <v>11756.0</v>
+        <v>11814.0</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>109</v>
@@ -21568,7 +21610,28 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="10"/>
+      <c r="A34" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B34" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" s="1">
+        <v>11756.0</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="10"/>
@@ -24503,6 +24566,9 @@
     </row>
     <row r="1012">
       <c r="A1012" s="10"/>
+    </row>
+    <row r="1013">
+      <c r="A1013" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -25168,20 +25234,17 @@
         <v>131</v>
       </c>
       <c r="B30" s="1">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="F30" s="1">
-        <v>12450.0</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>132</v>
+        <v>12746.0</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>33</v>
@@ -25202,10 +25265,10 @@
         <v>31</v>
       </c>
       <c r="F31" s="1">
-        <v>12500.0</v>
+        <v>12450.0</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>33</v>
@@ -25216,7 +25279,7 @@
         <v>131</v>
       </c>
       <c r="B32" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>31</v>
@@ -25226,17 +25289,38 @@
         <v>31</v>
       </c>
       <c r="F32" s="1">
-        <v>12600.0</v>
+        <v>12500.0</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="10"/>
+      <c r="A33" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B33" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F33" s="1">
+        <v>12600.0</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="10"/>
@@ -28183,6 +28267,9 @@
     </row>
     <row r="1015">
       <c r="A1015" s="10"/>
+    </row>
+    <row r="1016">
+      <c r="A1016" s="10"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -28479,38 +28566,38 @@
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B11" s="1">
         <v>3.0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F11" s="1">
-        <v>13738.0</v>
+        <v>2355.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B12" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F12" s="1">
-        <v>5039.0</v>
+        <v>13738.0</v>
       </c>
     </row>
     <row r="13">
@@ -28518,33 +28605,28 @@
         <v>146</v>
       </c>
       <c r="B13" s="1">
-        <v>7.0</v>
+        <v>4.0</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>93</v>
-      </c>
+      <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F13" s="1">
-        <v>4237.0</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>147</v>
+        <v>5039.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B14" s="1">
-        <v>2.0</v>
+        <v>7.0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>93</v>
@@ -28553,30 +28635,35 @@
         <v>25</v>
       </c>
       <c r="F14" s="1">
-        <v>1508.0</v>
+        <v>4237.0</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B15" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="E15" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F15" s="1">
-        <v>2343.0</v>
+        <v>1508.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B16" s="1">
         <v>1.0</v>
@@ -28589,43 +28676,46 @@
         <v>25</v>
       </c>
       <c r="F16" s="1">
-        <v>1440.0</v>
+        <v>2343.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B17" s="1">
-        <v>7.0</v>
+        <v>1.0</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F17" s="1">
-        <v>1613.0</v>
+        <v>5217.0</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B18" s="1">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F18" s="1">
-        <v>3554.0</v>
+        <v>2413.0</v>
       </c>
     </row>
     <row r="19">
@@ -28633,20 +28723,17 @@
         <v>151</v>
       </c>
       <c r="B19" s="1">
-        <v>8.0</v>
+        <v>1.0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F19" s="1">
-        <v>1608.0</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>136</v>
+        <v>1440.0</v>
       </c>
     </row>
     <row r="20">
@@ -28664,38 +28751,33 @@
         <v>16</v>
       </c>
       <c r="F20" s="1">
-        <v>2552.0</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>152</v>
+        <v>1613.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B21" s="1">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>93</v>
-      </c>
+      <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F21" s="1">
-        <v>2411.0</v>
+        <v>3554.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B22" s="1">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>16</v>
@@ -28705,149 +28787,134 @@
         <v>16</v>
       </c>
       <c r="F22" s="1">
-        <v>2849.0</v>
+        <v>1608.0</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B23" s="1">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>154</v>
+        <v>16</v>
       </c>
       <c r="F23" s="1">
-        <v>3557.0</v>
+        <v>2552.0</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B24" s="1">
         <v>6.0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="E24" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F24" s="1">
-        <v>2545.0</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>156</v>
+        <v>2411.0</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="B25" s="5">
-        <v>4.0</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="E25" s="6" t="s">
+      <c r="A25" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B25" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F25" s="5">
-        <v>2912.0</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="8"/>
-      <c r="R25" s="8"/>
-      <c r="S25" s="8"/>
-      <c r="T25" s="8"/>
-      <c r="U25" s="8"/>
-      <c r="V25" s="8"/>
-      <c r="W25" s="8"/>
-      <c r="X25" s="8"/>
-      <c r="Y25" s="8"/>
-      <c r="Z25" s="8"/>
-      <c r="AA25" s="8"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="1">
+        <v>2849.0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B26" s="1">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
-        <v>15</v>
+        <v>155</v>
       </c>
       <c r="F26" s="1">
-        <v>2553.0</v>
+        <v>3557.0</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B27" s="1">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="F27" s="1">
-        <v>5244.0</v>
+        <v>2545.0</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B28" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="5">
+        <v>2912.0</v>
+      </c>
+      <c r="G28" s="7" t="s">
         <v>158</v>
-      </c>
-      <c r="B28" s="5">
-        <v>6.0</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F28" s="5">
-        <v>4430.0</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>159</v>
       </c>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
@@ -28871,366 +28938,449 @@
       <c r="AA28" s="8"/>
     </row>
     <row r="29">
-      <c r="A29" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="B29" s="5">
+      <c r="A29" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B29" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="1">
+        <v>2553.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B30" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" s="1">
+        <v>5144.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B31" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" s="1">
+        <v>5244.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B32" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" s="5">
+        <v>4430.0</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
+      <c r="R32" s="8"/>
+      <c r="S32" s="8"/>
+      <c r="T32" s="8"/>
+      <c r="U32" s="8"/>
+      <c r="V32" s="8"/>
+      <c r="W32" s="8"/>
+      <c r="X32" s="8"/>
+      <c r="Y32" s="8"/>
+      <c r="Z32" s="8"/>
+      <c r="AA32" s="8"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B33" s="5">
         <v>8.0</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C33" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6" t="s">
+      <c r="D33" s="6"/>
+      <c r="E33" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F33" s="5">
         <v>3610.0</v>
       </c>
-      <c r="G29" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="8"/>
-      <c r="R29" s="8"/>
-      <c r="S29" s="8"/>
-      <c r="T29" s="8"/>
-      <c r="U29" s="8"/>
-      <c r="V29" s="8"/>
-      <c r="W29" s="8"/>
-      <c r="X29" s="8"/>
-      <c r="Y29" s="8"/>
-      <c r="Z29" s="8"/>
-      <c r="AA29" s="8"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="B30" s="5">
+      <c r="G33" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
+      <c r="Q33" s="8"/>
+      <c r="R33" s="8"/>
+      <c r="S33" s="8"/>
+      <c r="T33" s="8"/>
+      <c r="U33" s="8"/>
+      <c r="V33" s="8"/>
+      <c r="W33" s="8"/>
+      <c r="X33" s="8"/>
+      <c r="Y33" s="8"/>
+      <c r="Z33" s="8"/>
+      <c r="AA33" s="8"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B34" s="5">
         <v>8.0</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C34" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6" t="s">
+      <c r="D34" s="6"/>
+      <c r="E34" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F30" s="5">
+      <c r="F34" s="5">
         <v>3221.0</v>
       </c>
-      <c r="G30" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
-      <c r="S30" s="8"/>
-      <c r="T30" s="8"/>
-      <c r="U30" s="8"/>
-      <c r="V30" s="8"/>
-      <c r="W30" s="8"/>
-      <c r="X30" s="8"/>
-      <c r="Y30" s="8"/>
-      <c r="Z30" s="8"/>
-      <c r="AA30" s="8"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="B31" s="5">
+      <c r="G34" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="8"/>
+      <c r="S34" s="8"/>
+      <c r="T34" s="8"/>
+      <c r="U34" s="8"/>
+      <c r="V34" s="8"/>
+      <c r="W34" s="8"/>
+      <c r="X34" s="8"/>
+      <c r="Y34" s="8"/>
+      <c r="Z34" s="8"/>
+      <c r="AA34" s="8"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B35" s="5">
         <v>7.0</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C35" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6" t="s">
+      <c r="D35" s="6"/>
+      <c r="E35" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F31" s="5">
+      <c r="F35" s="5">
         <v>4300.0</v>
       </c>
-      <c r="G31" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="8"/>
-      <c r="T31" s="8"/>
-      <c r="U31" s="8"/>
-      <c r="V31" s="8"/>
-      <c r="W31" s="8"/>
-      <c r="X31" s="8"/>
-      <c r="Y31" s="8"/>
-      <c r="Z31" s="8"/>
-      <c r="AA31" s="8"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="B32" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F32" s="1">
-        <v>4059.0</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="B33" s="1">
-        <v>7.0</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F33" s="1">
-        <v>3407.0</v>
-      </c>
-      <c r="G33" s="1" t="s">
+      <c r="G35" s="9" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="B34" s="1">
-        <v>7.0</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F34" s="1">
-        <v>3625.0</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="B35" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F35" s="1">
-        <v>3621.0</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>165</v>
-      </c>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="8"/>
+      <c r="R35" s="8"/>
+      <c r="S35" s="8"/>
+      <c r="T35" s="8"/>
+      <c r="U35" s="8"/>
+      <c r="V35" s="8"/>
+      <c r="W35" s="8"/>
+      <c r="X35" s="8"/>
+      <c r="Y35" s="8"/>
+      <c r="Z35" s="8"/>
+      <c r="AA35" s="8"/>
     </row>
     <row r="36">
       <c r="A36" s="3" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B36" s="1">
-        <v>7.0</v>
+        <v>4.0</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="F36" s="1">
-        <v>3140.0</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>166</v>
+        <v>4059.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="3" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B37" s="1">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F37" s="1">
-        <v>3512.0</v>
+        <v>3407.0</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="3" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B38" s="1">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>154</v>
+        <v>33</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1" t="s">
-        <v>154</v>
+        <v>31</v>
       </c>
       <c r="F38" s="1">
-        <v>3332.0</v>
+        <v>3625.0</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B39" s="1">
         <v>6.0</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F39" s="1">
-        <v>3737.0</v>
+        <v>3621.0</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B40" s="1">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>93</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D40" s="1"/>
       <c r="E40" s="1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="F40" s="1">
-        <v>1500.0</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>169</v>
+        <v>3140.0</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B41" s="1">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F41" s="1">
-        <v>21150.0</v>
+        <v>3512.0</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B42" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>15</v>
+        <v>155</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F42" s="1">
+        <v>3332.0</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B43" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43" s="1">
+        <v>3737.0</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B44" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F44" s="1">
+        <v>1500.0</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B45" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F42" s="1">
+      <c r="F45" s="1">
+        <v>21150.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B46" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F46" s="1">
         <v>20943.0</v>
       </c>
-      <c r="G42" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="10"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="10"/>
-    </row>
-    <row r="45">
-      <c r="A45" s="10"/>
-    </row>
-    <row r="46">
-      <c r="A46" s="10"/>
+      <c r="G46" s="1" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="10"/>
@@ -32162,6 +32312,18 @@
     </row>
     <row r="1023">
       <c r="A1023" s="10"/>
+    </row>
+    <row r="1024">
+      <c r="A1024" s="10"/>
+    </row>
+    <row r="1025">
+      <c r="A1025" s="10"/>
+    </row>
+    <row r="1026">
+      <c r="A1026" s="10"/>
+    </row>
+    <row r="1027">
+      <c r="A1027" s="10"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -32209,7 +32371,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B2" s="1">
         <v>2.0</v>
@@ -32225,7 +32387,7 @@
         <v>14630.0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>8</v>
@@ -32233,7 +32395,7 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B3" s="1">
         <v>2.0</v>
@@ -32252,7 +32414,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B4" s="1">
         <v>4.0</v>
@@ -32271,7 +32433,7 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B5" s="1">
         <v>2.0</v>
@@ -32287,12 +32449,12 @@
         <v>1618.0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B6" s="1">
         <v>4.0</v>
@@ -32310,7 +32472,7 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B7" s="1">
         <v>5.0</v>
@@ -32328,7 +32490,7 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B8" s="1">
         <v>7.0</v>
@@ -32351,7 +32513,7 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B9" s="1">
         <v>7.0</v>
@@ -32372,7 +32534,7 @@
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B10" s="1">
         <v>6.0</v>
@@ -32388,22 +32550,22 @@
         <v>2303.0</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B11" s="1">
         <v>5.0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F11" s="1">
         <v>2431.0</v>
@@ -32411,7 +32573,7 @@
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B12" s="11">
         <v>5.0</v>
@@ -32427,7 +32589,7 @@
         <v>2532.0</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
@@ -32452,7 +32614,7 @@
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B13" s="1">
         <v>7.0</v>
@@ -32468,12 +32630,12 @@
         <v>2454.0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B14" s="5">
         <v>5.0</v>
@@ -32489,7 +32651,7 @@
         <v>3408.0</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H14" s="13"/>
       <c r="I14" s="8"/>
@@ -32514,7 +32676,7 @@
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B15" s="5">
         <v>5.0</v>
@@ -32530,7 +32692,7 @@
         <v>3912.0</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H15" s="13"/>
       <c r="I15" s="8"/>
@@ -32555,19 +32717,19 @@
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B16" s="1">
         <v>4.0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>93</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F16" s="1">
         <v>3849.0</v>
@@ -32575,7 +32737,7 @@
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B17" s="1">
         <v>6.0</v>
@@ -32591,12 +32753,12 @@
         <v>3915.0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B18" s="1">
         <v>4.0</v>
@@ -32612,12 +32774,12 @@
         <v>4249.0</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B19" s="1">
         <v>5.0</v>
@@ -32633,12 +32795,12 @@
         <v>4109.0</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B20" s="1">
         <v>5.0</v>
@@ -32656,12 +32818,12 @@
         <v>4045.0</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B21" s="1">
         <v>7.0</v>
@@ -32680,12 +32842,12 @@
         <v>18</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B22" s="1">
         <v>2.0</v>
@@ -32704,17 +32866,17 @@
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B23" s="1">
         <v>2.0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F23" s="1">
         <v>11526.0</v>
@@ -32723,7 +32885,7 @@
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B24" s="1">
         <v>4.0</v>
@@ -32739,12 +32901,12 @@
         <v>10330.0</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B25" s="1">
         <v>5.0</v>
@@ -32760,12 +32922,12 @@
         <v>10114.0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B26" s="1">
         <v>6.0</v>
@@ -32781,12 +32943,12 @@
         <v>10000.0</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B27" s="1">
         <v>7.0</v>
@@ -32804,17 +32966,17 @@
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B28" s="1">
         <v>5.0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F28" s="1">
         <v>5150.0</v>
@@ -32822,7 +32984,7 @@
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B29" s="1">
         <v>9.0</v>
@@ -32838,15 +33000,15 @@
         <v>5135.0</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="I29" s="15" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B30" s="1">
         <v>7.0</v>
@@ -32862,7 +33024,7 @@
         <v>10321.0</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="31">

</xml_diff>

<commit_message>
update graph to include all level permutations instead of just one with the hashmap
</commit_message>
<xml_diff>
--- a/data/times.xlsx
+++ b/data/times.xlsx
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1095" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="247">
   <si>
     <t>This spreadsheet is intended to capture all times for levels given some input and expected output.</t>
   </si>
@@ -726,6 +726,9 @@
     <t>7-7,7-8</t>
   </si>
   <si>
+    <t>skipping hands for now</t>
+  </si>
+  <si>
     <t>compare routing given nspade spawning on 3-6, getting cloud in 3-7, etc against what youd otherwise do with the same routing</t>
   </si>
   <si>
@@ -1910,6 +1913,9 @@
         <v>175</v>
       </c>
       <c r="C72" s="10"/>
+      <c r="D72" s="1" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="3" t="s">
@@ -1934,7 +1940,7 @@
         <v>180</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>93</v>
@@ -6653,12 +6659,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -6666,42 +6672,42 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>217</v>
-      </c>
       <c r="K4" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5">
@@ -6712,7 +6718,7 @@
         <v>2.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E5" s="1">
         <v>0.0</v>
@@ -6721,7 +6727,7 @@
         <v>2.0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="I5" s="1">
         <v>0.0</v>
@@ -6730,7 +6736,7 @@
         <v>2.0</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6">
@@ -6741,7 +6747,7 @@
         <v>2.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E6" s="1">
         <v>2.0</v>
@@ -6750,7 +6756,7 @@
         <v>2.0</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I6" s="1">
         <v>2.0</v>
@@ -6759,7 +6765,7 @@
         <v>2.0</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7">
@@ -6770,7 +6776,7 @@
         <v>12.0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E7" s="1">
         <v>12.0</v>
@@ -6779,7 +6785,7 @@
         <v>12.0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="I7" s="1">
         <v>12.0</v>
@@ -6788,7 +6794,7 @@
         <v>12.0</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8">
@@ -6799,7 +6805,7 @@
         <v>13.0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E8" s="1">
         <v>13.0</v>
@@ -6808,7 +6814,7 @@
         <v>13.0</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="I8" s="1">
         <v>11.0</v>
@@ -6817,7 +6823,7 @@
         <v>11.0</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9">
@@ -6828,7 +6834,7 @@
         <v>-8.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E9" s="1">
         <v>-10.0</v>
@@ -6837,7 +6843,7 @@
         <v>-8.0</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="I9" s="1">
         <v>-10.0</v>
@@ -6846,7 +6852,7 @@
         <v>-8.0</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10">
@@ -6857,7 +6863,7 @@
         <v>30.5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E10" s="1">
         <v>30.5</v>
@@ -6866,7 +6872,7 @@
         <v>30.5</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="I10" s="1">
         <v>30.5</v>
@@ -6875,7 +6881,7 @@
         <v>30.5</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11">
@@ -6886,7 +6892,7 @@
         <v>25.5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E11" s="1">
         <v>25.5</v>
@@ -6895,7 +6901,7 @@
         <v>25.5</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="I11" s="1">
         <v>25.5</v>
@@ -6904,7 +6910,7 @@
         <v>25.5</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12">
@@ -6915,7 +6921,7 @@
         <v>1.0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E12" s="1">
         <v>1.0</v>
@@ -6924,7 +6930,7 @@
         <v>1.0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13">
@@ -6935,7 +6941,7 @@
         <v>-3.0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E13" s="1">
         <v>-3.0</v>
@@ -6944,7 +6950,7 @@
         <v>-3.0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14">
@@ -6955,7 +6961,7 @@
         <v>-1.5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E14" s="1">
         <v>-1.5</v>
@@ -6964,7 +6970,7 @@
         <v>-1.5</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15">
@@ -6975,7 +6981,7 @@
         <v>1.0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E15" s="1">
         <v>1.0</v>
@@ -6984,7 +6990,7 @@
         <v>1.0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I15" s="1">
         <v>1.0</v>
@@ -6993,7 +6999,7 @@
         <v>1.0</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16">
@@ -7004,7 +7010,7 @@
         <v>-3.0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E16" s="1">
         <v>-3.0</v>
@@ -7013,7 +7019,7 @@
         <v>-3.0</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="I16" s="1">
         <v>-3.0</v>
@@ -7022,7 +7028,7 @@
         <v>-3.0</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="17">
@@ -7033,7 +7039,7 @@
         <v>-2.0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E17" s="1">
         <v>-2.0</v>
@@ -7042,7 +7048,7 @@
         <v>-2.0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18">
@@ -7053,7 +7059,7 @@
         <v>-1.0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E18" s="1">
         <v>-1.0</v>
@@ -7062,7 +7068,7 @@
         <v>-1.0</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="I18" s="1">
         <v>-1.0</v>
@@ -7071,7 +7077,7 @@
         <v>-1.0</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="19">
@@ -7082,7 +7088,7 @@
         <v>-36.25</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E19" s="1">
         <v>-36.0</v>
@@ -7091,10 +7097,10 @@
         <v>-36.0</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="I19" s="1">
         <v>-36.25</v>
@@ -7103,7 +7109,7 @@
         <v>-36.25</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="20">
@@ -7114,7 +7120,7 @@
         <v>-41.0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E20" s="1">
         <v>-40.5</v>
@@ -7123,7 +7129,7 @@
         <v>-40.5</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="I20" s="1">
         <v>-41.0</v>
@@ -7132,7 +7138,7 @@
         <v>-41.0</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="21">
@@ -7145,7 +7151,7 @@
         <v>-8.75</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E21" s="16">
         <f t="shared" ref="E21:F21" si="2">SUM(E5:E20)</f>
@@ -7156,7 +7162,7 @@
         <v>-8</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I21" s="16">
         <f t="shared" ref="I21:J21" si="3">sum(I5:I20)</f>
@@ -7167,7 +7173,7 @@
         <v>-5.25</v>
       </c>
       <c r="K21" s="17" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -7198,15 +7204,15 @@
   <sheetData>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B3" s="1">
         <v>16.0</v>
@@ -7214,7 +7220,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B4" s="1">
         <v>17.0</v>
@@ -7222,7 +7228,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B5" s="1">
         <f>86-20</f>
@@ -7231,7 +7237,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B6" s="18">
         <f>92+1</f>
@@ -7240,7 +7246,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B7" s="18">
         <f>1817-1785</f>
@@ -7249,7 +7255,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B8" s="1">
         <v>37.0</v>
@@ -7257,7 +7263,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B9" s="18">
         <f>4*60</f>
@@ -24888,20 +24894,20 @@
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B15" s="1">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F15" s="1">
-        <v>1626.0</v>
+        <v>2112.0</v>
       </c>
     </row>
     <row r="16">
@@ -24909,41 +24915,38 @@
         <v>122</v>
       </c>
       <c r="B16" s="1">
-        <v>7.0</v>
+        <v>1.0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F16" s="1">
-        <v>1511.0</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>123</v>
+        <v>1626.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B17" s="1">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F17" s="1">
-        <v>2724.0</v>
+        <v>1511.0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18">
@@ -24951,7 +24954,7 @@
         <v>124</v>
       </c>
       <c r="B18" s="1">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>31</v>
@@ -24961,10 +24964,10 @@
         <v>31</v>
       </c>
       <c r="F18" s="1">
-        <v>2502.0</v>
+        <v>2724.0</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19">
@@ -24972,7 +24975,7 @@
         <v>124</v>
       </c>
       <c r="B19" s="1">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>31</v>
@@ -24982,52 +24985,32 @@
         <v>31</v>
       </c>
       <c r="F19" s="1">
+        <v>2502.0</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="1">
         <v>2244.0</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B20" s="11">
-        <v>7.0</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" s="5">
-        <v>2606.0</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="8"/>
-      <c r="T20" s="8"/>
-      <c r="U20" s="8"/>
-      <c r="V20" s="8"/>
-      <c r="W20" s="8"/>
-      <c r="X20" s="8"/>
-      <c r="Y20" s="8"/>
-      <c r="Z20" s="8"/>
-      <c r="AA20" s="8"/>
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
@@ -25037,14 +25020,14 @@
         <v>7.0</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="6" t="s">
         <v>31</v>
       </c>
       <c r="F21" s="5">
-        <v>2434.0</v>
+        <v>2606.0</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>74</v>
@@ -25071,45 +25054,65 @@
       <c r="AA21" s="8"/>
     </row>
     <row r="22">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B22" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="1">
-        <v>2215.0</v>
-      </c>
-      <c r="G22" s="1" t="s">
+      <c r="B22" s="11">
+        <v>7.0</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="5">
+        <v>2434.0</v>
+      </c>
+      <c r="G22" s="7" t="s">
         <v>74</v>
       </c>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+      <c r="T22" s="8"/>
+      <c r="U22" s="8"/>
+      <c r="V22" s="8"/>
+      <c r="W22" s="8"/>
+      <c r="X22" s="8"/>
+      <c r="Y22" s="8"/>
+      <c r="Z22" s="8"/>
+      <c r="AA22" s="8"/>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B23" s="1">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F23" s="1">
-        <v>3640.0</v>
+        <v>2215.0</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>129</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24">
@@ -25117,7 +25120,7 @@
         <v>128</v>
       </c>
       <c r="B24" s="1">
-        <v>8.0</v>
+        <v>4.0</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>25</v>
@@ -25127,10 +25130,10 @@
         <v>16</v>
       </c>
       <c r="F24" s="1">
-        <v>2932.0</v>
+        <v>3640.0</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25">
@@ -25138,17 +25141,20 @@
         <v>128</v>
       </c>
       <c r="B25" s="1">
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="F25" s="1">
-        <v>3337.0</v>
+        <v>2932.0</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="26">
@@ -25159,14 +25165,14 @@
         <v>4.0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="F26" s="1">
-        <v>4014.0</v>
+        <v>3337.0</v>
       </c>
     </row>
     <row r="27">
@@ -25181,10 +25187,10 @@
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F27" s="1">
-        <v>3715.0</v>
+        <v>4014.0</v>
       </c>
     </row>
     <row r="28">
@@ -25192,7 +25198,7 @@
         <v>128</v>
       </c>
       <c r="B28" s="1">
-        <v>8.0</v>
+        <v>4.0</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>15</v>
@@ -25202,31 +25208,28 @@
         <v>15</v>
       </c>
       <c r="F28" s="1">
-        <v>2909.0</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>130</v>
+        <v>3715.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B29" s="1">
-        <v>2.0</v>
+        <v>8.0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F29" s="1">
-        <v>12716.0</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>33</v>
+        <v>2909.0</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="30">
@@ -25237,14 +25240,14 @@
         <v>2.0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F30" s="1">
-        <v>12746.0</v>
+        <v>12716.0</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>33</v>
@@ -25255,20 +25258,17 @@
         <v>131</v>
       </c>
       <c r="B31" s="1">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="F31" s="1">
-        <v>12450.0</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>132</v>
+        <v>12746.0</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>33</v>
@@ -25289,10 +25289,10 @@
         <v>31</v>
       </c>
       <c r="F32" s="1">
-        <v>12500.0</v>
+        <v>12450.0</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>33</v>
@@ -25303,7 +25303,7 @@
         <v>131</v>
       </c>
       <c r="B33" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>31</v>
@@ -25313,17 +25313,38 @@
         <v>31</v>
       </c>
       <c r="F33" s="1">
-        <v>12600.0</v>
+        <v>12500.0</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="10"/>
+      <c r="A34" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" s="1">
+        <v>12600.0</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="10"/>
@@ -28270,6 +28291,9 @@
     </row>
     <row r="1016">
       <c r="A1016" s="10"/>
+    </row>
+    <row r="1017">
+      <c r="A1017" s="10"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -28583,90 +28607,104 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B12" s="1">
+      <c r="A12" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B12" s="11">
         <v>3.0</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="1">
-        <v>13738.0</v>
-      </c>
+      <c r="C12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="5">
+        <v>2425.0</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="8"/>
+      <c r="Y12" s="8"/>
+      <c r="Z12" s="8"/>
+      <c r="AA12" s="8"/>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B13" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F13" s="1">
-        <v>5039.0</v>
+        <v>13738.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B14" s="1">
-        <v>7.0</v>
+        <v>3.0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>93</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="F14" s="1">
-        <v>4237.0</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>147</v>
+        <v>13738.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B15" s="1">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>93</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F15" s="1">
-        <v>1508.0</v>
+        <v>13738.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B16" s="1">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>33</v>
@@ -28676,51 +28714,55 @@
         <v>25</v>
       </c>
       <c r="F16" s="1">
-        <v>2343.0</v>
+        <v>5039.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B17" s="1">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="E17" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F17" s="1">
-        <v>5217.0</v>
+        <v>4237.0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B18" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="E18" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F18" s="1">
-        <v>2413.0</v>
+        <v>1508.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B19" s="1">
         <v>1.0</v>
@@ -28733,209 +28775,202 @@
         <v>25</v>
       </c>
       <c r="F19" s="1">
-        <v>1440.0</v>
+        <v>2343.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B20" s="1">
-        <v>7.0</v>
+        <v>1.0</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="1">
+        <v>5217.0</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B21" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="1">
-        <v>1613.0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B21" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="6"/>
+      <c r="E21" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" s="1">
-        <v>3554.0</v>
-      </c>
+      <c r="F21" s="5">
+        <v>5247.0</v>
+      </c>
+      <c r="G21" s="14"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+      <c r="T21" s="8"/>
+      <c r="U21" s="8"/>
+      <c r="V21" s="8"/>
+      <c r="W21" s="8"/>
+      <c r="X21" s="8"/>
+      <c r="Y21" s="8"/>
+      <c r="Z21" s="8"/>
+      <c r="AA21" s="8"/>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B22" s="1">
-        <v>8.0</v>
+        <v>1.0</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F22" s="1">
-        <v>1608.0</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>136</v>
+        <v>2413.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B23" s="1">
-        <v>7.0</v>
+        <v>1.0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F23" s="1">
-        <v>2552.0</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>153</v>
+        <v>1440.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B24" s="1">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>93</v>
-      </c>
+      <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F24" s="1">
-        <v>2411.0</v>
+        <v>1613.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B25" s="1">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F25" s="1">
-        <v>2849.0</v>
+        <v>3554.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B26" s="1">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
-        <v>155</v>
+        <v>16</v>
       </c>
       <c r="F26" s="1">
-        <v>3557.0</v>
+        <v>1608.0</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B27" s="1">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F27" s="1">
-        <v>2545.0</v>
+        <v>2552.0</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B28" s="5">
-        <v>4.0</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D28" s="9" t="s">
+      <c r="B28" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E28" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F28" s="5">
-        <v>2912.0</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
-      <c r="T28" s="8"/>
-      <c r="U28" s="8"/>
-      <c r="V28" s="8"/>
-      <c r="W28" s="8"/>
-      <c r="X28" s="8"/>
-      <c r="Y28" s="8"/>
-      <c r="Z28" s="8"/>
-      <c r="AA28" s="8"/>
+      <c r="F28" s="1">
+        <v>2411.0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
@@ -28945,19 +28980,19 @@
         <v>6.0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F29" s="1">
-        <v>2553.0</v>
+        <v>2849.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B30" s="1">
         <v>5.0</v>
@@ -28967,49 +29002,57 @@
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
-        <v>16</v>
+        <v>155</v>
       </c>
       <c r="F30" s="1">
-        <v>5144.0</v>
+        <v>3557.0</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B31" s="1">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="F31" s="1">
-        <v>5244.0</v>
+        <v>2545.0</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="4" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B32" s="5">
-        <v>6.0</v>
-      </c>
-      <c r="C32" s="6" t="s">
+        <v>4.0</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6" t="s">
-        <v>31</v>
-      </c>
       <c r="F32" s="5">
-        <v>4430.0</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>160</v>
+        <v>2912.0</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>158</v>
       </c>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
@@ -29033,270 +29076,281 @@
       <c r="AA32" s="8"/>
     </row>
     <row r="33">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B33" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="1">
+        <v>2553.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B34" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" s="1">
+        <v>5144.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B35" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F35" s="1">
+        <v>5244.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B36" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F36" s="5">
+        <v>4430.0</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8"/>
+      <c r="R36" s="8"/>
+      <c r="S36" s="8"/>
+      <c r="T36" s="8"/>
+      <c r="U36" s="8"/>
+      <c r="V36" s="8"/>
+      <c r="W36" s="8"/>
+      <c r="X36" s="8"/>
+      <c r="Y36" s="8"/>
+      <c r="Z36" s="8"/>
+      <c r="AA36" s="8"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B37" s="5">
         <v>8.0</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C37" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6" t="s">
+      <c r="D37" s="6"/>
+      <c r="E37" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F33" s="5">
+      <c r="F37" s="5">
         <v>3610.0</v>
       </c>
-      <c r="G33" s="9" t="s">
+      <c r="G37" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
-      <c r="R33" s="8"/>
-      <c r="S33" s="8"/>
-      <c r="T33" s="8"/>
-      <c r="U33" s="8"/>
-      <c r="V33" s="8"/>
-      <c r="W33" s="8"/>
-      <c r="X33" s="8"/>
-      <c r="Y33" s="8"/>
-      <c r="Z33" s="8"/>
-      <c r="AA33" s="8"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="4" t="s">
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="8"/>
+      <c r="R37" s="8"/>
+      <c r="S37" s="8"/>
+      <c r="T37" s="8"/>
+      <c r="U37" s="8"/>
+      <c r="V37" s="8"/>
+      <c r="W37" s="8"/>
+      <c r="X37" s="8"/>
+      <c r="Y37" s="8"/>
+      <c r="Z37" s="8"/>
+      <c r="AA37" s="8"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B38" s="5">
         <v>8.0</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C38" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6" t="s">
+      <c r="D38" s="6"/>
+      <c r="E38" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F34" s="5">
+      <c r="F38" s="5">
         <v>3221.0</v>
       </c>
-      <c r="G34" s="9" t="s">
+      <c r="G38" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="8"/>
-      <c r="Q34" s="8"/>
-      <c r="R34" s="8"/>
-      <c r="S34" s="8"/>
-      <c r="T34" s="8"/>
-      <c r="U34" s="8"/>
-      <c r="V34" s="8"/>
-      <c r="W34" s="8"/>
-      <c r="X34" s="8"/>
-      <c r="Y34" s="8"/>
-      <c r="Z34" s="8"/>
-      <c r="AA34" s="8"/>
-    </row>
-    <row r="35">
-      <c r="A35" s="4" t="s">
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="8"/>
+      <c r="S38" s="8"/>
+      <c r="T38" s="8"/>
+      <c r="U38" s="8"/>
+      <c r="V38" s="8"/>
+      <c r="W38" s="8"/>
+      <c r="X38" s="8"/>
+      <c r="Y38" s="8"/>
+      <c r="Z38" s="8"/>
+      <c r="AA38" s="8"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B39" s="5">
         <v>7.0</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C39" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6" t="s">
+      <c r="D39" s="6"/>
+      <c r="E39" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F35" s="5">
+      <c r="F39" s="5">
         <v>4300.0</v>
       </c>
-      <c r="G35" s="9" t="s">
+      <c r="G39" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="8"/>
-      <c r="S35" s="8"/>
-      <c r="T35" s="8"/>
-      <c r="U35" s="8"/>
-      <c r="V35" s="8"/>
-      <c r="W35" s="8"/>
-      <c r="X35" s="8"/>
-      <c r="Y35" s="8"/>
-      <c r="Z35" s="8"/>
-      <c r="AA35" s="8"/>
-    </row>
-    <row r="36">
-      <c r="A36" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B36" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F36" s="1">
-        <v>4059.0</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B37" s="1">
-        <v>7.0</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F37" s="1">
-        <v>3407.0</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B38" s="1">
-        <v>7.0</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F38" s="1">
-        <v>3625.0</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B39" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F39" s="1">
-        <v>3621.0</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>166</v>
-      </c>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
+      <c r="S39" s="8"/>
+      <c r="T39" s="8"/>
+      <c r="U39" s="8"/>
+      <c r="V39" s="8"/>
+      <c r="W39" s="8"/>
+      <c r="X39" s="8"/>
+      <c r="Y39" s="8"/>
+      <c r="Z39" s="8"/>
+      <c r="AA39" s="8"/>
     </row>
     <row r="40">
       <c r="A40" s="3" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B40" s="1">
-        <v>7.0</v>
+        <v>4.0</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="F40" s="1">
-        <v>3140.0</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>167</v>
+        <v>4059.0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B41" s="1">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F41" s="1">
-        <v>3512.0</v>
+        <v>3407.0</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B42" s="1">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>155</v>
+        <v>33</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1" t="s">
-        <v>155</v>
+        <v>31</v>
       </c>
       <c r="F42" s="1">
-        <v>3332.0</v>
+        <v>3625.0</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="43">
@@ -29307,14 +29361,14 @@
         <v>6.0</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F43" s="1">
-        <v>3737.0</v>
+        <v>3621.0</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>166</v>
@@ -29322,83 +29376,191 @@
     </row>
     <row r="44">
       <c r="A44" s="3" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B44" s="1">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>93</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D44" s="1"/>
       <c r="E44" s="1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="F44" s="1">
-        <v>1500.0</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>170</v>
+        <v>3140.0</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B45" s="1">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F45" s="1">
-        <v>21150.0</v>
+        <v>3512.0</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B46" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>15</v>
+        <v>155</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F46" s="1">
+        <v>3332.0</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B47" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F47" s="1">
+        <v>3737.0</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B48" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F48" s="1">
+        <v>1500.0</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B49" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F46" s="1">
+      <c r="F49" s="1">
+        <v>21150.0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B50" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F50" s="1">
         <v>20943.0</v>
       </c>
-      <c r="G46" s="1" t="s">
+      <c r="G50" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" s="10"/>
-    </row>
-    <row r="48">
-      <c r="A48" s="10"/>
-    </row>
-    <row r="49">
-      <c r="A49" s="10"/>
-    </row>
-    <row r="50">
-      <c r="A50" s="10"/>
-    </row>
     <row r="51">
-      <c r="A51" s="10"/>
+      <c r="A51" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B51" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F51" s="1">
+        <v>20913.0</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="52">
-      <c r="A52" s="10"/>
+      <c r="A52" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B52" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F52" s="1">
+        <v>20843.0</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="10"/>
@@ -32324,6 +32486,21 @@
     </row>
     <row r="1027">
       <c r="A1027" s="10"/>
+    </row>
+    <row r="1028">
+      <c r="A1028" s="10"/>
+    </row>
+    <row r="1029">
+      <c r="A1029" s="10"/>
+    </row>
+    <row r="1030">
+      <c r="A1030" s="10"/>
+    </row>
+    <row r="1031">
+      <c r="A1031" s="10"/>
+    </row>
+    <row r="1032">
+      <c r="A1032" s="10"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>